<commit_message>
Revisi Kondisi Rumah off
</commit_message>
<xml_diff>
--- a/Rekap/RekapKondisiRumah.xlsx
+++ b/Rekap/RekapKondisiRumah.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Bangunan Tinggal" sheetId="1" r:id="rId1"/>
@@ -1315,9 +1315,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -1358,7 +1358,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1372,13 +1417,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1387,39 +1434,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1442,10 +1457,25 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1470,36 +1500,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1510,7 +1510,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1522,31 +1564,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1558,19 +1582,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1588,7 +1600,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1612,7 +1642,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1624,73 +1684,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1728,15 +1728,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1748,6 +1739,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1790,44 +1816,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1839,130 +1839,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2324,7 +2324,7 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2986,7 +2986,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C3:G27;C2:G2" numberStoredAsText="1"/>
+    <ignoredError sqref="C2:G2;C3:G27" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6892,8 +6892,8 @@
   <sheetPr/>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -6983,13 +6983,13 @@
         <v>14</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>233</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>10</v>
@@ -7029,10 +7029,10 @@
         <v>20</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>10</v>
@@ -7532,7 +7532,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C2:G27" numberStoredAsText="1"/>
+    <ignoredError sqref="C4:E4;F4:G4;C2:G3;C5:G5;C6:G6;C7:G27" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>